<commit_message>
added equipment carbon dioxide emissions report
</commit_message>
<xml_diff>
--- a/myems-normalization/data_repair_sample.xlsx
+++ b/myems-normalization/data_repair_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>计量表对应的能耗值点ID，每个文件仅支持一个数据点ID，如果需要补录多个数据点，请创建多个文件分别上传</t>
+    <r>
+      <t>计量表对应的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>能耗值点</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID，每个文件仅支持一个数据点ID，如果需要补录多个数据点，请创建多个文件分别上传</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -463,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
@@ -719,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>